<commit_message>
Import NCC to Misa
</commit_message>
<xml_diff>
--- a/Output/Danh muc NCC mau.xlsx
+++ b/Output/Danh muc NCC mau.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\UiPath\Project path\Amber_MuaHang_Vlookup\Output\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\UiPath\Project path\Amber\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53F2B509-46A3-45BD-AB73-C6C95E9A17E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62DB1119-F2F5-447A-B564-9B5CB53EB5EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,9 +17,6 @@
     <sheet name="Danh mục cũ" sheetId="2" r:id="rId2"/>
     <sheet name="Danh mục cập nhật" sheetId="3" r:id="rId3"/>
   </sheets>
-  <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Danh mục mới'!$A$1:$G$52</definedName>
-  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -41,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="514" uniqueCount="288">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="512" uniqueCount="288">
   <si>
     <t>Mã nhà cung cấp (*)</t>
   </si>
@@ -1034,7 +1031,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1065,12 +1062,13 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="49" fontId="2" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection hidden="1"/>
@@ -1359,11 +1357,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <sheetPr filterMode="1"/>
-  <dimension ref="A1:G52"/>
+  <dimension ref="A1:F52"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:B50"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1376,7 +1373,7 @@
     <col min="6" max="6" width="16.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1396,626 +1393,415 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="22.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" ht="22.8" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>21</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>253</v>
       </c>
-      <c r="G2" t="str">
-        <f>VLOOKUP(A2,'Danh mục cũ'!$F$2:$F$79,1,0)</f>
-        <v>0101159195</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>24</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>254</v>
       </c>
-      <c r="G3" t="str">
-        <f>VLOOKUP(A3,'Danh mục cũ'!$F$2:$F$79,1,0)</f>
-        <v>0101360697</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" ht="22.8" hidden="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="4" spans="1:6" ht="22.8" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
         <v>168</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>169</v>
       </c>
-      <c r="G4" t="str">
-        <f>VLOOKUP(A4,'Danh mục cũ'!$F$2:$F$79,1,0)</f>
-        <v>0108683721</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" ht="22.8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="5" spans="1:6" ht="22.8" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
         <v>251</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>255</v>
       </c>
-      <c r="G5" t="e">
-        <f>VLOOKUP(A5,'Danh mục cũ'!$F$2:$F$79,1,0)</f>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
         <v>247</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>256</v>
       </c>
-      <c r="G6" t="e">
-        <f>VLOOKUP(A6,'Danh mục cũ'!$F$2:$F$79,1,0)</f>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" ht="22.8" hidden="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="7" spans="1:6" ht="22.8" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
         <v>202</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>257</v>
       </c>
-      <c r="G7" t="str">
-        <f>VLOOKUP(A7,'Danh mục cũ'!$F$2:$F$79,1,0)</f>
-        <v>0310439453-001</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" ht="34.200000000000003" hidden="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="8" spans="1:6" ht="34.200000000000003" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
         <v>26</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="G8" t="str">
-        <f>VLOOKUP(A8,'Danh mục cũ'!$F$2:$F$79,1,0)</f>
-        <v>0101507727-001</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" ht="22.8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="9" spans="1:6" ht="22.8" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
         <v>240</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>258</v>
       </c>
-      <c r="G9" t="e">
-        <f>VLOOKUP(A9,'Danh mục cũ'!$F$2:$F$79,1,0)</f>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" ht="22.8" hidden="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="10" spans="1:6" ht="22.8" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
         <v>99</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>259</v>
       </c>
-      <c r="G10" t="str">
-        <f>VLOOKUP(A10,'Danh mục cũ'!$F$2:$F$79,1,0)</f>
-        <v>0106136096</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" ht="22.8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="11" spans="1:6" ht="22.8" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="s">
         <v>252</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>260</v>
       </c>
-      <c r="G11" t="e">
-        <f>VLOOKUP(A11,'Danh mục cũ'!$F$2:$F$79,1,0)</f>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" s="4" t="s">
         <v>73</v>
       </c>
       <c r="B12" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="G12" t="str">
-        <f>VLOOKUP(A12,'Danh mục cũ'!$F$2:$F$79,1,0)</f>
-        <v>0104789847</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" s="4" t="s">
         <v>139</v>
       </c>
       <c r="B13" s="3" t="s">
         <v>140</v>
       </c>
-      <c r="G13" t="str">
-        <f>VLOOKUP(A13,'Danh mục cũ'!$F$2:$F$79,1,0)</f>
-        <v>0107486248</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" ht="22.8" hidden="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="14" spans="1:6" ht="22.8" x14ac:dyDescent="0.3">
       <c r="A14" s="4" t="s">
         <v>116</v>
       </c>
       <c r="B14" s="3" t="s">
         <v>117</v>
       </c>
-      <c r="G14" t="str">
-        <f>VLOOKUP(A14,'Danh mục cũ'!$F$2:$F$79,1,0)</f>
-        <v>0106765288</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" ht="22.8" hidden="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="15" spans="1:6" ht="22.8" x14ac:dyDescent="0.3">
       <c r="A15" s="4" t="s">
         <v>199</v>
       </c>
       <c r="B15" s="3" t="s">
         <v>200</v>
       </c>
-      <c r="G15" t="str">
-        <f>VLOOKUP(A15,'Danh mục cũ'!$F$2:$F$79,1,0)</f>
-        <v>0305616442</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" s="4" t="s">
         <v>185</v>
       </c>
       <c r="B16" s="3" t="s">
         <v>186</v>
       </c>
-      <c r="G16" t="str">
-        <f>VLOOKUP(A16,'Danh mục cũ'!$F$2:$F$79,1,0)</f>
-        <v>0109534271</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" s="4" t="s">
         <v>88</v>
       </c>
       <c r="B17" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="G17" t="str">
-        <f>VLOOKUP(A17,'Danh mục cũ'!$F$2:$F$79,1,0)</f>
-        <v>0105670033</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" ht="22.8" hidden="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="18" spans="1:2" ht="22.8" x14ac:dyDescent="0.3">
       <c r="A18" s="4" t="s">
         <v>53</v>
       </c>
       <c r="B18" s="3" t="s">
         <v>261</v>
       </c>
-      <c r="G18" t="str">
-        <f>VLOOKUP(A18,'Danh mục cũ'!$F$2:$F$79,1,0)</f>
-        <v>0102755063</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" s="4" t="s">
         <v>41</v>
       </c>
       <c r="B19" s="3" t="s">
         <v>262</v>
       </c>
-      <c r="G19" t="str">
-        <f>VLOOKUP(A19,'Danh mục cũ'!$F$2:$F$79,1,0)</f>
-        <v>0102343655</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" ht="34.200000000000003" x14ac:dyDescent="0.3">
+    </row>
+    <row r="20" spans="1:2" ht="34.200000000000003" x14ac:dyDescent="0.3">
       <c r="A20" s="4" t="s">
         <v>249</v>
       </c>
       <c r="B20" s="3" t="s">
         <v>263</v>
       </c>
-      <c r="G20" t="e">
-        <f>VLOOKUP(A20,'Danh mục cũ'!$F$2:$F$79,1,0)</f>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" ht="22.8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="21" spans="1:2" ht="22.8" x14ac:dyDescent="0.3">
       <c r="A21" s="4" t="s">
         <v>248</v>
       </c>
       <c r="B21" s="3" t="s">
         <v>264</v>
       </c>
-      <c r="G21" t="e">
-        <f>VLOOKUP(A21,'Danh mục cũ'!$F$2:$F$79,1,0)</f>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" s="4" t="s">
         <v>151</v>
       </c>
       <c r="B22" s="3" t="s">
         <v>152</v>
       </c>
-      <c r="G22" t="str">
-        <f>VLOOKUP(A22,'Danh mục cũ'!$F$2:$F$79,1,0)</f>
-        <v>0107864972</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" ht="22.8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="23" spans="1:2" ht="22.8" x14ac:dyDescent="0.3">
       <c r="A23" s="4" t="s">
         <v>244</v>
       </c>
       <c r="B23" s="3" t="s">
         <v>265</v>
       </c>
-      <c r="G23" t="e">
-        <f>VLOOKUP(A23,'Danh mục cũ'!$F$2:$F$79,1,0)</f>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" ht="22.8" hidden="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="24" spans="1:2" ht="22.8" x14ac:dyDescent="0.3">
       <c r="A24" s="4" t="s">
         <v>82</v>
       </c>
       <c r="B24" s="3" t="s">
         <v>266</v>
       </c>
-      <c r="G24" t="str">
-        <f>VLOOKUP(A24,'Danh mục cũ'!$F$2:$F$79,1,0)</f>
-        <v>0105283179</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" ht="22.8" hidden="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="25" spans="1:2" ht="22.8" x14ac:dyDescent="0.3">
       <c r="A25" s="4" t="s">
         <v>93</v>
       </c>
       <c r="B25" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="G25" t="str">
-        <f>VLOOKUP(A25,'Danh mục cũ'!$F$2:$F$79,1,0)</f>
-        <v>0105957237</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" s="4" t="s">
         <v>148</v>
       </c>
       <c r="B26" s="3" t="s">
         <v>267</v>
       </c>
-      <c r="G26" t="str">
-        <f>VLOOKUP(A26,'Danh mục cũ'!$F$2:$F$79,1,0)</f>
-        <v>0107762787</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27" s="4" t="s">
         <v>159</v>
       </c>
       <c r="B27" s="3" t="s">
         <v>160</v>
       </c>
-      <c r="G27" t="str">
-        <f>VLOOKUP(A27,'Danh mục cũ'!$F$2:$F$79,1,0)</f>
-        <v>0108386863</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" ht="22.8" hidden="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="28" spans="1:2" ht="22.8" x14ac:dyDescent="0.3">
       <c r="A28" s="4" t="s">
         <v>226</v>
       </c>
       <c r="B28" s="3" t="s">
         <v>268</v>
       </c>
-      <c r="G28" t="str">
-        <f>VLOOKUP(A28,'Danh mục cũ'!$F$2:$F$79,1,0)</f>
-        <v>0500570248</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" ht="22.8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="29" spans="1:2" ht="22.8" x14ac:dyDescent="0.3">
       <c r="A29" s="4" t="s">
         <v>245</v>
       </c>
       <c r="B29" s="3" t="s">
         <v>269</v>
       </c>
-      <c r="G29" t="e">
-        <f>VLOOKUP(A29,'Danh mục cũ'!$F$2:$F$79,1,0)</f>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" ht="22.8" hidden="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="30" spans="1:2" ht="22.8" x14ac:dyDescent="0.3">
       <c r="A30" s="4" t="s">
         <v>35</v>
       </c>
       <c r="B30" s="3" t="s">
         <v>270</v>
       </c>
-      <c r="G30" t="str">
-        <f>VLOOKUP(A30,'Danh mục cũ'!$F$2:$F$79,1,0)</f>
-        <v>0102190423</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A31" s="4" t="s">
         <v>180</v>
       </c>
       <c r="B31" s="3" t="s">
         <v>181</v>
       </c>
-      <c r="G31" t="str">
-        <f>VLOOKUP(A31,'Danh mục cũ'!$F$2:$F$79,1,0)</f>
-        <v>0108995054</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" ht="22.8" hidden="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="32" spans="1:2" ht="22.8" x14ac:dyDescent="0.3">
       <c r="A32" s="4" t="s">
         <v>177</v>
       </c>
       <c r="B32" s="3" t="s">
         <v>178</v>
       </c>
-      <c r="G32" t="str">
-        <f>VLOOKUP(A32,'Danh mục cũ'!$F$2:$F$79,1,0)</f>
-        <v>0108915796</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" ht="22.8" hidden="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="33" spans="1:2" ht="22.8" x14ac:dyDescent="0.3">
       <c r="A33" s="4" t="s">
         <v>133</v>
       </c>
       <c r="B33" s="3" t="s">
         <v>134</v>
       </c>
-      <c r="G33" t="str">
-        <f>VLOOKUP(A33,'Danh mục cũ'!$F$2:$F$79,1,0)</f>
-        <v>0107322095</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7" ht="22.8" hidden="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="34" spans="1:2" ht="22.8" x14ac:dyDescent="0.3">
       <c r="A34" s="4" t="s">
         <v>119</v>
       </c>
       <c r="B34" s="3" t="s">
         <v>271</v>
       </c>
-      <c r="G34" t="str">
-        <f>VLOOKUP(A34,'Danh mục cũ'!$F$2:$F$79,1,0)</f>
-        <v>0106768200</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A35" s="4" t="s">
         <v>241</v>
       </c>
       <c r="B35" s="3" t="s">
         <v>272</v>
       </c>
-      <c r="G35" t="e">
-        <f>VLOOKUP(A35,'Danh mục cũ'!$F$2:$F$79,1,0)</f>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A36" s="4" t="s">
         <v>238</v>
       </c>
       <c r="B36" s="3" t="s">
         <v>273</v>
       </c>
-      <c r="G36" t="e">
-        <f>VLOOKUP(A36,'Danh mục cũ'!$F$2:$F$79,1,0)</f>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7" ht="22.8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="37" spans="1:2" ht="22.8" x14ac:dyDescent="0.3">
       <c r="A37" s="4" t="s">
         <v>243</v>
       </c>
       <c r="B37" s="3" t="s">
         <v>274</v>
       </c>
-      <c r="G37" t="e">
-        <f>VLOOKUP(A37,'Danh mục cũ'!$F$2:$F$79,1,0)</f>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7" ht="22.8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="38" spans="1:2" ht="22.8" x14ac:dyDescent="0.3">
       <c r="A38" s="4" t="s">
         <v>242</v>
       </c>
       <c r="B38" s="3" t="s">
         <v>275</v>
       </c>
-      <c r="G38" t="e">
-        <f>VLOOKUP(A38,'Danh mục cũ'!$F$2:$F$79,1,0)</f>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A39" s="4" t="s">
         <v>250</v>
       </c>
       <c r="B39" s="3" t="s">
         <v>276</v>
       </c>
-      <c r="G39" t="e">
-        <f>VLOOKUP(A39,'Danh mục cũ'!$F$2:$F$79,1,0)</f>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A40" s="4" t="s">
         <v>246</v>
       </c>
       <c r="B40" s="3" t="s">
         <v>277</v>
       </c>
-      <c r="G40" t="e">
-        <f>VLOOKUP(A40,'Danh mục cũ'!$F$2:$F$79,1,0)</f>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="41" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A41" s="4" t="s">
         <v>57</v>
       </c>
       <c r="B41" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="G41" t="str">
-        <f>VLOOKUP(A41,'Danh mục cũ'!$F$2:$F$79,1,0)</f>
-        <v>0103867884</v>
-      </c>
-    </row>
-    <row r="42" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A42" s="4" t="s">
         <v>208</v>
       </c>
       <c r="B42" s="3" t="s">
         <v>278</v>
       </c>
-      <c r="G42" t="str">
-        <f>VLOOKUP(A42,'Danh mục cũ'!$F$2:$F$79,1,0)</f>
-        <v>0312002637</v>
-      </c>
-    </row>
-    <row r="43" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A43" s="4" t="s">
         <v>110</v>
       </c>
       <c r="B43" s="3" t="s">
         <v>279</v>
       </c>
-      <c r="G43" t="str">
-        <f>VLOOKUP(A43,'Danh mục cũ'!$F$2:$F$79,1,0)</f>
-        <v>0106696387</v>
-      </c>
-    </row>
-    <row r="44" spans="1:7" ht="22.8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="44" spans="1:2" ht="22.8" x14ac:dyDescent="0.3">
       <c r="A44" s="4" t="s">
         <v>237</v>
       </c>
       <c r="B44" s="3" t="s">
         <v>280</v>
       </c>
-      <c r="G44" t="e">
-        <f>VLOOKUP(A44,'Danh mục cũ'!$F$2:$F$79,1,0)</f>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="45" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A45" s="4" t="s">
         <v>11</v>
       </c>
       <c r="B45" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="G45" t="str">
-        <f>VLOOKUP(A45,'Danh mục cũ'!$F$2:$F$79,1,0)</f>
-        <v>0100101114-042</v>
-      </c>
-    </row>
-    <row r="46" spans="1:7" ht="22.8" hidden="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="46" spans="1:2" ht="22.8" x14ac:dyDescent="0.3">
       <c r="A46" s="4" t="s">
         <v>127</v>
       </c>
       <c r="B46" s="3" t="s">
         <v>281</v>
       </c>
-      <c r="G46" t="str">
-        <f>VLOOKUP(A46,'Danh mục cũ'!$F$2:$F$79,1,0)</f>
-        <v>0106869738-002</v>
-      </c>
-    </row>
-    <row r="47" spans="1:7" ht="22.8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="47" spans="1:2" ht="22.8" x14ac:dyDescent="0.3">
       <c r="A47" s="4" t="s">
         <v>236</v>
       </c>
       <c r="B47" s="3" t="s">
         <v>282</v>
       </c>
-      <c r="G47" t="e">
-        <f>VLOOKUP(A47,'Danh mục cũ'!$F$2:$F$79,1,0)</f>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="48" spans="1:7" ht="22.8" hidden="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="48" spans="1:2" ht="22.8" x14ac:dyDescent="0.3">
       <c r="A48" s="4" t="s">
         <v>104</v>
       </c>
       <c r="B48" s="3" t="s">
         <v>283</v>
       </c>
-      <c r="G48" t="str">
-        <f>VLOOKUP(A48,'Danh mục cũ'!$F$2:$F$79,1,0)</f>
-        <v>0106488901</v>
-      </c>
-    </row>
-    <row r="49" spans="1:7" ht="22.8" hidden="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="49" spans="1:2" ht="22.8" x14ac:dyDescent="0.3">
       <c r="A49" s="4" t="s">
         <v>18</v>
       </c>
       <c r="B49" s="3" t="s">
         <v>284</v>
       </c>
-      <c r="G49" t="str">
-        <f>VLOOKUP(A49,'Danh mục cũ'!$F$2:$F$79,1,0)</f>
-        <v>0100956381</v>
-      </c>
-    </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A50" s="4" t="s">
         <v>239</v>
       </c>
       <c r="B50" s="3" t="s">
         <v>285</v>
       </c>
-      <c r="G50" t="e">
-        <f>VLOOKUP(A50,'Danh mục cũ'!$F$2:$F$79,1,0)</f>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="51" spans="1:7" ht="22.8" hidden="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="51" spans="1:2" ht="22.8" x14ac:dyDescent="0.3">
       <c r="A51" s="4" t="s">
         <v>190</v>
       </c>
       <c r="B51" s="3" t="s">
         <v>286</v>
       </c>
-      <c r="G51" t="str">
-        <f>VLOOKUP(A51,'Danh mục cũ'!$F$2:$F$79,1,0)</f>
-        <v>0302249586-001</v>
-      </c>
-    </row>
-    <row r="52" spans="1:7" ht="22.8" hidden="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="52" spans="1:2" ht="22.8" x14ac:dyDescent="0.3">
       <c r="A52" s="4" t="s">
         <v>188</v>
       </c>
       <c r="B52" s="3" t="s">
         <v>287</v>
       </c>
-      <c r="G52" t="str">
-        <f>VLOOKUP(A52,'Danh mục cũ'!$F$2:$F$79,1,0)</f>
-        <v>0300792451-004</v>
-      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:G52" xr:uid="{00000000-0001-0000-0000-000000000000}">
-    <filterColumn colId="6">
-      <filters>
-        <filter val="#N/A"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
   <dataValidations count="2">
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Nếu 1 nhà cung cấp thuộc nhiều nhóm KH vui lòng phân cách mã nhóm bằng dấu ;" sqref="E1" xr:uid="{74092DF5-69A0-48E9-AC0A-AB8202BEE9D1}">
       <formula1>0</formula1>
@@ -3884,109 +3670,106 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01D51B57-DEC2-4BA9-A98C-5DAC0771ED9E}">
-  <dimension ref="A1:F51"/>
+  <dimension ref="A1:F52"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="23.77734375" customWidth="1"/>
-    <col min="2" max="2" width="27.33203125" customWidth="1"/>
-    <col min="3" max="3" width="15.109375" customWidth="1"/>
-    <col min="4" max="4" width="15.6640625" customWidth="1"/>
-    <col min="5" max="5" width="20" customWidth="1"/>
-    <col min="6" max="6" width="22.5546875" customWidth="1"/>
+    <col min="1" max="1" width="23.77734375" style="12" customWidth="1"/>
+    <col min="2" max="2" width="27.33203125" style="12" customWidth="1"/>
+    <col min="3" max="3" width="15.109375" style="12" customWidth="1"/>
+    <col min="4" max="4" width="15.6640625" style="12" customWidth="1"/>
+    <col min="5" max="5" width="20" style="12" customWidth="1"/>
+    <col min="6" max="6" width="22.5546875" style="12" customWidth="1"/>
+    <col min="7" max="16384" width="8.88671875" style="12"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A1" s="12" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="12" t="s">
+    <row r="1" spans="1:6" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A1" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="12" t="s">
+      <c r="C1" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="12" t="s">
+      <c r="D1" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="13" t="s">
+      <c r="E1" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="13" t="s">
+      <c r="F1" s="14" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="22.8" x14ac:dyDescent="0.3">
-      <c r="A2" s="4" t="s">
-        <v>247</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>256</v>
-      </c>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" s="10"/>
+      <c r="B2" s="11"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A3" s="4"/>
-      <c r="B3" s="3"/>
+      <c r="A3" s="10"/>
+      <c r="B3" s="11"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A4" s="4"/>
-      <c r="B4" s="3"/>
+      <c r="A4" s="10"/>
+      <c r="B4" s="11"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A5" s="4"/>
-      <c r="B5" s="3"/>
+      <c r="A5" s="10"/>
+      <c r="B5" s="11"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A6" s="4"/>
-      <c r="B6" s="3"/>
+      <c r="A6" s="10"/>
+      <c r="B6" s="11"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A7" s="4"/>
-      <c r="B7" s="3"/>
+      <c r="A7" s="10"/>
+      <c r="B7" s="11"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A8" s="4"/>
-      <c r="B8" s="3"/>
+      <c r="A8" s="10"/>
+      <c r="B8" s="11"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A9" s="4"/>
-      <c r="B9" s="3"/>
+      <c r="A9" s="10"/>
+      <c r="B9" s="11"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A10" s="4"/>
-      <c r="B10" s="3"/>
+      <c r="A10" s="10"/>
+      <c r="B10" s="11"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A11" s="4"/>
-      <c r="B11" s="3"/>
+      <c r="A11" s="10"/>
+      <c r="B11" s="11"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A12" s="4"/>
-      <c r="B12" s="3"/>
+      <c r="A12" s="10"/>
+      <c r="B12" s="11"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A13" s="4"/>
-      <c r="B13" s="3"/>
+      <c r="A13" s="10"/>
+      <c r="B13" s="11"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A14" s="4"/>
-      <c r="B14" s="3"/>
+      <c r="A14" s="10"/>
+      <c r="B14" s="11"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A15" s="4"/>
-      <c r="B15" s="3"/>
+      <c r="A15" s="10"/>
+      <c r="B15" s="11"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A16" s="4"/>
-      <c r="B16" s="3"/>
+      <c r="A16" s="10"/>
+      <c r="B16" s="11"/>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A17" s="4"/>
-      <c r="B17" s="3"/>
+      <c r="A17" s="10"/>
+      <c r="B17" s="11"/>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" s="10"/>
@@ -4123,6 +3906,10 @@
     <row r="51" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A51" s="10"/>
       <c r="B51" s="11"/>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A52" s="10"/>
+      <c r="B52" s="11"/>
     </row>
   </sheetData>
   <dataValidations count="2">

</xml_diff>

<commit_message>
fix loi tinh trang
</commit_message>
<xml_diff>
--- a/Output/Danh muc NCC mau.xlsx
+++ b/Output/Danh muc NCC mau.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\RPA_Amber_MuaHang\Output\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\JOB\RPA Project\RPA_AmberMuaHang\Output\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99FFBE77-2B7D-461D-9206-EA24F5BEDCCB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D92495B2-DEFB-44FA-A6DA-6D8D53E0B3A9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2448" yWindow="360" windowWidth="17820" windowHeight="11436" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Danh mục mới'!$A$1:$G$1</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="179021"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -405,7 +405,7 @@
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:G147"/>
+      <selection activeCell="A2" sqref="A2:G45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -501,7 +501,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:G1" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <autoFilter ref="A1:G1" xr:uid="{4B9A0918-F2C7-4B4C-A4B5-FC3816D76855}">
     <filterColumn colId="6">
       <filters blank="1"/>
     </filterColumn>

</xml_diff>